<commit_message>
change the label in the forest plot for paper revision
</commit_message>
<xml_diff>
--- a/analysis/forest_plot_nsaid.xlsx
+++ b/analysis/forest_plot_nsaid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20363"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20369"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\COVID19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nsaids-covid-research\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC76F17-2817-43E1-81D7-C685A48DED34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7270ABC-D752-4A3D-9CF6-1534E6687090}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="3555" windowHeight="3930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="3555" windowHeight="3930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nsaid_population" sheetId="7" r:id="rId1"/>
@@ -41,15 +41,9 @@
     <t>{bf:Main analysis}</t>
   </si>
   <si>
-    <t>Univariable</t>
-  </si>
-  <si>
     <t>Age/sex adjusted</t>
   </si>
   <si>
-    <t>Fully adjusted</t>
-  </si>
-  <si>
     <t>{bf:Other analysis: COX-2 specific}</t>
   </si>
   <si>
@@ -75,6 +69,12 @@
   </si>
   <si>
     <t>Ibuprofen</t>
+  </si>
+  <si>
+    <t>Unadjusted</t>
+  </si>
+  <si>
+    <t>Multivariable-adjusted</t>
   </si>
 </sst>
 </file>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +478,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -498,19 +498,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3">
-        <v>1.25</v>
+        <v>1.26</v>
       </c>
       <c r="D2" s="3">
-        <v>1.07</v>
+        <v>1.08</v>
       </c>
       <c r="E2" s="3">
-        <v>1.46</v>
+        <v>1.47</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>5</v>
@@ -518,19 +518,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3">
-        <v>1.08</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="D3" s="3">
-        <v>0.93</v>
+        <v>0.94</v>
       </c>
       <c r="E3" s="3">
-        <v>1.27</v>
+        <v>1.28</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
@@ -538,19 +538,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="D4" s="3">
         <v>0.8</v>
       </c>
       <c r="E4" s="3">
-        <v>1.1299999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>5</v>
@@ -558,133 +558,133 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3">
-        <v>1.32</v>
+        <v>1.4</v>
       </c>
       <c r="D5" s="3">
-        <v>0.98</v>
+        <v>1.05</v>
       </c>
       <c r="E5" s="3">
-        <v>1.77</v>
+        <v>1.87</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="D6" s="3">
-        <v>0.74</v>
+        <v>0.73</v>
       </c>
       <c r="E6" s="3">
-        <v>1.1599999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3">
-        <v>1.02</v>
+        <v>1.08</v>
       </c>
       <c r="D7" s="3">
-        <v>0.76</v>
+        <v>0.81</v>
       </c>
       <c r="E7" s="3">
-        <v>1.37</v>
+        <v>1.44</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3">
-        <v>1.07</v>
+        <v>1.05</v>
       </c>
       <c r="D8" s="3">
-        <v>0.85</v>
+        <v>0.84</v>
       </c>
       <c r="E8" s="3">
-        <v>1.34</v>
+        <v>1.32</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.87</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.64</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.19</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.17</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.93</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.73</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.19</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C11" s="3">
-        <v>1.1200000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="D11" s="3">
         <v>0.57999999999999996</v>
@@ -693,18 +693,18 @@
         <v>2.15</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3">
-        <v>0.76</v>
+        <v>0.77</v>
       </c>
       <c r="D12" s="3">
         <v>0.4</v>
@@ -713,15 +713,15 @@
         <v>1.48</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C13" s="3">
         <v>0.61</v>
@@ -733,15 +733,15 @@
         <v>1.18</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3">
         <v>2.79</v>
@@ -750,38 +750,38 @@
         <v>2.0699999999999998</v>
       </c>
       <c r="E14" s="3">
-        <v>3.77</v>
+        <v>3.76</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="3">
-        <v>1.34</v>
+        <v>1.35</v>
       </c>
       <c r="D15" s="3">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="E15" s="3">
-        <v>1.81</v>
+        <v>1.82</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C16" s="3">
         <v>1.23</v>
@@ -790,10 +790,10 @@
         <v>0.9</v>
       </c>
       <c r="E16" s="3">
-        <v>1.67</v>
+        <v>1.68</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -806,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +819,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -839,10 +839,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3">
         <v>0.43</v>
@@ -859,16 +859,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3">
-        <v>0.84</v>
+        <v>0.83</v>
       </c>
       <c r="D3" s="3">
-        <v>0.7</v>
+        <v>0.69</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -879,16 +879,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3">
         <v>0.78</v>
       </c>
       <c r="D4" s="3">
-        <v>0.65</v>
+        <v>0.64</v>
       </c>
       <c r="E4" s="3">
         <v>0.94</v>
@@ -899,133 +899,133 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3">
-        <v>0.46</v>
+        <v>0.49</v>
       </c>
       <c r="D5" s="3">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
       <c r="E5" s="3">
-        <v>0.68</v>
+        <v>0.71</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3">
-        <v>0.34</v>
+        <v>0.33</v>
       </c>
       <c r="D6" s="3">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="E6" s="3">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3">
-        <v>0.78</v>
+        <v>0.83</v>
       </c>
       <c r="D7" s="3">
-        <v>0.53</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E7" s="3">
-        <v>1.1399999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3">
-        <v>0.87</v>
+        <v>0.85</v>
       </c>
       <c r="D8" s="3">
-        <v>0.65</v>
+        <v>0.63</v>
       </c>
       <c r="E8" s="3">
-        <v>1.18</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.77</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.72</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.49</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.05</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.07</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.81</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C11" s="3">
-        <v>0.3</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D11" s="3">
         <v>0.13</v>
@@ -1034,18 +1034,18 @@
         <v>0.66</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3">
-        <v>0.56999999999999995</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D12" s="3">
         <v>0.25</v>
@@ -1054,87 +1054,87 @@
         <v>1.26</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C13" s="3">
-        <v>0.49</v>
+        <v>0.48</v>
       </c>
       <c r="D13" s="3">
         <v>0.22</v>
       </c>
       <c r="E13" s="3">
-        <v>1.0900000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3">
-        <v>0.71</v>
+        <v>0.68</v>
       </c>
       <c r="D14" s="3">
-        <v>0.48</v>
+        <v>0.45</v>
       </c>
       <c r="E14" s="3">
-        <v>1.05</v>
+        <v>1.01</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="3">
-        <v>0.88</v>
+        <v>0.85</v>
       </c>
       <c r="D15" s="3">
-        <v>0.6</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E15" s="3">
-        <v>1.31</v>
+        <v>1.27</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="C16" s="3">
-        <v>0.87</v>
+        <v>0.83</v>
       </c>
       <c r="D16" s="3">
-        <v>0.59</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="E16" s="3">
-        <v>1.3</v>
+        <v>1.25</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>